<commit_message>
add Goldsmith 2003 JCR
</commit_message>
<xml_diff>
--- a/manuscript/Empirical Strategies Summary.xlsx
+++ b/manuscript/Empirical Strategies Summary.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkalley14\Dropbox\Research\Dissertation\arms-allies-review\manuscript\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="186">
   <si>
     <t>Authors</t>
   </si>
@@ -559,6 +564,24 @@
   </si>
   <si>
     <t>W/S, number of rivals, capabilities, MIDS in PRIE</t>
+  </si>
+  <si>
+    <t>Goldsmith</t>
+  </si>
+  <si>
+    <t>OLS: PCSE</t>
+  </si>
+  <si>
+    <t>Expendityres / GDP</t>
+  </si>
+  <si>
+    <t>Dummy: Defense Pact</t>
+  </si>
+  <si>
+    <t>1886-1989</t>
+  </si>
+  <si>
+    <t>GDP, regime type, lagged DV, war, rivalries, regional context, major power, systemic variables</t>
   </si>
 </sst>
 </file>
@@ -868,7 +891,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -876,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,122 +1248,113 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="B9">
-        <v>1990</v>
+        <v>2003</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>182</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>183</v>
       </c>
       <c r="H9" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="I9" t="s">
-        <v>72</v>
+        <v>184</v>
       </c>
       <c r="J9" t="s">
-        <v>84</v>
+        <v>16</v>
+      </c>
+      <c r="K9" t="s">
+        <v>185</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
-      </c>
-      <c r="M9" t="s">
-        <v>26</v>
-      </c>
-      <c r="N9" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B10">
-        <v>2017</v>
+        <v>1990</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="E10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="I10" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="J10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="L10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M10" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N10" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>176</v>
+        <v>85</v>
       </c>
       <c r="B11">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="G11" t="s">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
       </c>
       <c r="I11" t="s">
-        <v>178</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
       </c>
       <c r="K11" t="s">
-        <v>179</v>
+        <v>90</v>
       </c>
       <c r="L11" t="s">
         <v>75</v>
@@ -1348,40 +1362,43 @@
       <c r="M11" t="s">
         <v>17</v>
       </c>
+      <c r="N11" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>176</v>
       </c>
       <c r="B12">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
       <c r="H12" t="s">
         <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="L12" t="s">
         <v>75</v>
@@ -1395,7 +1412,7 @@
         <v>139</v>
       </c>
       <c r="B13">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
@@ -1404,22 +1421,25 @@
         <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>86</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="J13" t="s">
-        <v>99</v>
+        <v>16</v>
+      </c>
+      <c r="K13" t="s">
+        <v>95</v>
       </c>
       <c r="L13" t="s">
         <v>75</v>
@@ -1427,166 +1447,163 @@
       <c r="M13" t="s">
         <v>17</v>
       </c>
-      <c r="N13" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="B14">
-        <v>1993</v>
+        <v>2003</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="J14" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="L14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M14" t="s">
         <v>17</v>
       </c>
       <c r="N14" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="B15">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F15" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="G15" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="I15" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="J15" t="s">
-        <v>109</v>
-      </c>
-      <c r="K15" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="L15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M15" t="s">
         <v>17</v>
       </c>
       <c r="N15" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B16">
-        <v>1966</v>
+        <v>1987</v>
       </c>
       <c r="C16" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F16" t="s">
-        <v>70</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H16" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16">
-        <v>1964</v>
+        <v>69</v>
+      </c>
+      <c r="I16" t="s">
+        <v>113</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>109</v>
+      </c>
+      <c r="K16" t="s">
+        <v>69</v>
       </c>
       <c r="L16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M16" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="N16" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B17">
-        <v>1996</v>
+        <v>1966</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>117</v>
       </c>
       <c r="F17" t="s">
         <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H17" t="s">
         <v>37</v>
       </c>
-      <c r="I17" t="s">
-        <v>119</v>
+      <c r="I17">
+        <v>1964</v>
       </c>
       <c r="J17" t="s">
-        <v>16</v>
-      </c>
-      <c r="K17" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="L17" t="s">
         <v>74</v>
@@ -1594,22 +1611,19 @@
       <c r="M17" t="s">
         <v>26</v>
       </c>
-      <c r="N17" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="B18">
-        <v>1990</v>
+        <v>1996</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E18" t="s">
         <v>41</v>
@@ -1618,19 +1632,19 @@
         <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H18" t="s">
         <v>37</v>
       </c>
       <c r="I18" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="J18" t="s">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="K18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L18" t="s">
         <v>74</v>
@@ -1639,203 +1653,209 @@
         <v>26</v>
       </c>
       <c r="N18" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B19">
-        <v>1999</v>
+        <v>1990</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="E19" t="s">
         <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H19" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>98</v>
+        <v>127</v>
       </c>
       <c r="J19" t="s">
-        <v>132</v>
+        <v>73</v>
+      </c>
+      <c r="K19" t="s">
+        <v>125</v>
       </c>
       <c r="L19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M19" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B20">
-        <v>2015</v>
+        <v>1999</v>
       </c>
       <c r="C20" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>130</v>
       </c>
       <c r="G20" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="I20" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
-      </c>
-      <c r="K20" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="L20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M20" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="N20" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B21">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C21" t="s">
         <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>146</v>
+        <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21">
-        <v>2000</v>
+        <v>36</v>
+      </c>
+      <c r="I21" t="s">
+        <v>143</v>
       </c>
       <c r="J21" t="s">
-        <v>149</v>
+        <v>73</v>
       </c>
       <c r="K21" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="L21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M21" t="s">
-        <v>17</v>
-      </c>
-      <c r="N21" t="s">
-        <v>150</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B22">
-        <v>1983</v>
+        <v>2011</v>
       </c>
       <c r="C22" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>70</v>
       </c>
       <c r="G22" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
-      </c>
-      <c r="I22" t="s">
-        <v>155</v>
+        <v>37</v>
+      </c>
+      <c r="I22">
+        <v>2000</v>
       </c>
       <c r="J22" t="s">
-        <v>154</v>
+        <v>149</v>
+      </c>
+      <c r="K22" t="s">
+        <v>147</v>
       </c>
       <c r="L22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M22" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="N22" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B23">
-        <v>2012</v>
+        <v>1983</v>
       </c>
       <c r="C23" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="D23" t="s">
         <v>22</v>
       </c>
       <c r="E23" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" t="s">
+        <v>153</v>
+      </c>
+      <c r="H23" t="s">
         <v>69</v>
       </c>
-      <c r="F23" t="s">
-        <v>70</v>
-      </c>
-      <c r="G23" t="s">
-        <v>160</v>
-      </c>
-      <c r="I23">
-        <v>1820</v>
+      <c r="I23" t="s">
+        <v>155</v>
       </c>
       <c r="J23" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L23" t="s">
         <v>74</v>
@@ -1844,118 +1864,118 @@
         <v>26</v>
       </c>
       <c r="N23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B24">
-        <v>1994</v>
+        <v>2012</v>
       </c>
       <c r="C24" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>69</v>
       </c>
       <c r="F24" t="s">
-        <v>163</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
-        <v>164</v>
-      </c>
-      <c r="H24" t="s">
-        <v>36</v>
-      </c>
-      <c r="I24" t="s">
-        <v>166</v>
+        <v>160</v>
+      </c>
+      <c r="I24">
+        <v>1820</v>
       </c>
       <c r="J24" t="s">
-        <v>167</v>
-      </c>
-      <c r="K24" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="L24" t="s">
         <v>74</v>
       </c>
       <c r="M24" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="N24" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B25">
-        <v>1974</v>
+        <v>1994</v>
       </c>
       <c r="C25" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
-        <v>130</v>
+        <v>163</v>
       </c>
       <c r="G25" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="H25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I25" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J25" t="s">
-        <v>154</v>
+        <v>167</v>
+      </c>
+      <c r="K25" t="s">
+        <v>165</v>
       </c>
       <c r="L25" t="s">
         <v>74</v>
       </c>
       <c r="M25" t="s">
-        <v>26</v>
-      </c>
-      <c r="N25" t="s">
-        <v>170</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B26">
-        <v>1987</v>
+        <v>1974</v>
       </c>
       <c r="C26" t="s">
-        <v>32</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="E26" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="F26" t="s">
         <v>130</v>
       </c>
       <c r="G26" t="s">
-        <v>174</v>
+        <v>153</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>37</v>
+      </c>
+      <c r="I26" t="s">
+        <v>169</v>
       </c>
       <c r="J26" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="L26" t="s">
         <v>74</v>
@@ -1964,6 +1984,44 @@
         <v>26</v>
       </c>
       <c r="N26" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>171</v>
+      </c>
+      <c r="B27">
+        <v>1987</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>130</v>
+      </c>
+      <c r="G27" t="s">
+        <v>174</v>
+      </c>
+      <c r="H27" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" t="s">
+        <v>172</v>
+      </c>
+      <c r="L27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M27" t="s">
+        <v>26</v>
+      </c>
+      <c r="N27" t="s">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Barnett and Levy 1991
</commit_message>
<xml_diff>
--- a/manuscript/Empirical Strategies Summary.xlsx
+++ b/manuscript/Empirical Strategies Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="189">
   <si>
     <t>Authors</t>
   </si>
@@ -218,9 +218,6 @@
     <t>ln(Military expenditures)</t>
   </si>
   <si>
-    <t>CONDITIONAL. Also, lots of different model specs and estimators show same result</t>
-  </si>
-  <si>
     <t>LDV, regime type, rivals, war, ln(GDP), peacetime coordination</t>
   </si>
   <si>
@@ -272,9 +269,6 @@
     <t>GDP, Conventional and Strategic spending</t>
   </si>
   <si>
-    <t>Military Spending</t>
-  </si>
-  <si>
     <t>Divides conventional and strategic spending</t>
   </si>
   <si>
@@ -572,9 +566,6 @@
     <t>OLS: PCSE</t>
   </si>
   <si>
-    <t>Expendityres / GDP</t>
-  </si>
-  <si>
     <t>Dummy: Defense Pact</t>
   </si>
   <si>
@@ -582,6 +573,24 @@
   </si>
   <si>
     <t>GDP, regime type, lagged DV, war, rivalries, regional context, major power, systemic variables</t>
+  </si>
+  <si>
+    <t>Barnett &amp; Levy</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>1962-73</t>
+  </si>
+  <si>
+    <t>Alignment</t>
+  </si>
+  <si>
+    <t>Economic Conditions</t>
+  </si>
+  <si>
+    <t>CONDITIONAL. Also robust, lots of different model specs and estimators show same result</t>
   </si>
 </sst>
 </file>
@@ -899,10 +908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,7 +965,7 @@
         <v>18</v>
       </c>
       <c r="L1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
@@ -1000,7 +1009,7 @@
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M2" t="s">
         <v>17</v>
@@ -1008,192 +1017,189 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>183</v>
       </c>
       <c r="B3">
-        <v>1996</v>
+        <v>1991</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>186</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>187</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>185</v>
       </c>
       <c r="J3" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="L3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B4">
-        <v>1994</v>
+        <v>1996</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M4" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="N4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="B5">
-        <v>1990</v>
+        <v>1994</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
         <v>74</v>
       </c>
       <c r="M5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B6">
-        <v>1994</v>
+        <v>1990</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>54</v>
-      </c>
-      <c r="K6" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B7">
-        <v>2016</v>
+        <v>1994</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
         <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="H7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="J7" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="K7" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
         <v>75</v>
@@ -1201,248 +1207,248 @@
       <c r="M7" t="s">
         <v>17</v>
       </c>
-      <c r="N7" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B8">
-        <v>1992</v>
+        <v>2016</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
       </c>
       <c r="I8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="J8" t="s">
-        <v>73</v>
+        <v>16</v>
+      </c>
+      <c r="K8" t="s">
+        <v>64</v>
       </c>
       <c r="L8" t="s">
         <v>74</v>
       </c>
       <c r="M8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>66</v>
       </c>
       <c r="B9">
-        <v>2003</v>
+        <v>1992</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>181</v>
+        <v>68</v>
       </c>
       <c r="F9" t="s">
-        <v>182</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>183</v>
+        <v>70</v>
       </c>
       <c r="H9" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="I9" t="s">
-        <v>184</v>
+        <v>71</v>
       </c>
       <c r="J9" t="s">
-        <v>16</v>
-      </c>
-      <c r="K9" t="s">
-        <v>185</v>
+        <v>72</v>
       </c>
       <c r="L9" t="s">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="M9" t="s">
+        <v>26</v>
+      </c>
+      <c r="N9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>178</v>
       </c>
       <c r="B10">
-        <v>1990</v>
+        <v>2003</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D10" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>80</v>
+        <v>179</v>
       </c>
       <c r="F10" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>180</v>
       </c>
       <c r="H10" t="s">
-        <v>133</v>
+        <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>16</v>
+      </c>
+      <c r="K10" t="s">
+        <v>182</v>
       </c>
       <c r="L10" t="s">
         <v>74</v>
       </c>
-      <c r="M10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N10" t="s">
-        <v>83</v>
-      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B11">
-        <v>2017</v>
+        <v>1990</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>114</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="I11" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="J11" t="s">
-        <v>16</v>
-      </c>
-      <c r="K11" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M11" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N11" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>83</v>
       </c>
       <c r="B12">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="G12" t="s">
-        <v>177</v>
+        <v>86</v>
       </c>
       <c r="H12" t="s">
         <v>37</v>
       </c>
       <c r="I12" t="s">
-        <v>178</v>
+        <v>87</v>
       </c>
       <c r="J12" t="s">
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>179</v>
+        <v>88</v>
       </c>
       <c r="L12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M12" t="s">
         <v>17</v>
       </c>
+      <c r="N12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="B13">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>175</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>92</v>
+        <v>176</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>95</v>
+        <v>177</v>
       </c>
       <c r="L13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M13" t="s">
         <v>17</v>
@@ -1450,10 +1456,10 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B14">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
@@ -1462,63 +1468,63 @@
         <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G14" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s">
         <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J14" t="s">
-        <v>99</v>
+        <v>16</v>
+      </c>
+      <c r="K14" t="s">
+        <v>93</v>
       </c>
       <c r="L14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M14" t="s">
         <v>17</v>
       </c>
-      <c r="N14" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="B15">
-        <v>1993</v>
+        <v>2003</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="J15" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="L15" t="s">
         <v>74</v>
@@ -1527,502 +1533,543 @@
         <v>17</v>
       </c>
       <c r="N15" t="s">
-        <v>107</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>138</v>
+        <v>98</v>
       </c>
       <c r="B16">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="G16" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="H16" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="J16" t="s">
-        <v>109</v>
-      </c>
-      <c r="K16" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
       <c r="L16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M16" t="s">
         <v>17</v>
       </c>
       <c r="N16" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B17">
-        <v>1966</v>
+        <v>1987</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>110</v>
+      </c>
+      <c r="H17" t="s">
         <v>68</v>
       </c>
-      <c r="E17" t="s">
-        <v>117</v>
-      </c>
-      <c r="F17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" t="s">
-        <v>118</v>
-      </c>
-      <c r="H17" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17">
-        <v>1964</v>
+      <c r="I17" t="s">
+        <v>111</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>107</v>
+      </c>
+      <c r="K17" t="s">
+        <v>68</v>
       </c>
       <c r="L17" t="s">
         <v>74</v>
       </c>
       <c r="M17" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="N17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18">
-        <v>1996</v>
+        <v>1966</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>41</v>
+        <v>115</v>
       </c>
       <c r="F18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H18" t="s">
         <v>37</v>
       </c>
-      <c r="I18" t="s">
-        <v>119</v>
+      <c r="I18">
+        <v>1964</v>
       </c>
       <c r="J18" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="L18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M18" t="s">
         <v>26</v>
       </c>
-      <c r="N18" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B19">
-        <v>1990</v>
+        <v>1996</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
         <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="H19" t="s">
         <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="J19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" t="s">
+        <v>119</v>
+      </c>
+      <c r="L19" t="s">
         <v>73</v>
-      </c>
-      <c r="K19" t="s">
-        <v>125</v>
-      </c>
-      <c r="L19" t="s">
-        <v>74</v>
       </c>
       <c r="M19" t="s">
         <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B20">
-        <v>1999</v>
+        <v>1990</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>22</v>
       </c>
       <c r="E20" t="s">
         <v>41</v>
       </c>
       <c r="F20" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="H20" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="I20" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>72</v>
+      </c>
+      <c r="K20" t="s">
+        <v>123</v>
       </c>
       <c r="L20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M20" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="N20" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B21">
-        <v>2015</v>
+        <v>1999</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>68</v>
+        <v>127</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
       </c>
       <c r="F21" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>131</v>
       </c>
       <c r="I21" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="J21" t="s">
-        <v>73</v>
-      </c>
-      <c r="K21" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="L21" t="s">
         <v>74</v>
       </c>
       <c r="M21" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="N21" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B22">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="C22" t="s">
+        <v>139</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" t="s">
         <v>141</v>
       </c>
-      <c r="D22" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" t="s">
-        <v>146</v>
-      </c>
-      <c r="F22" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" t="s">
-        <v>148</v>
-      </c>
-      <c r="H22" t="s">
-        <v>37</v>
-      </c>
-      <c r="I22">
-        <v>2000</v>
-      </c>
       <c r="J22" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="K22" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="L22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M22" t="s">
-        <v>17</v>
-      </c>
-      <c r="N22" t="s">
-        <v>150</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B23">
-        <v>1983</v>
+        <v>2011</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F23" t="s">
-        <v>130</v>
+        <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" t="s">
-        <v>155</v>
+        <v>37</v>
+      </c>
+      <c r="I23">
+        <v>2000</v>
       </c>
       <c r="J23" t="s">
-        <v>154</v>
+        <v>147</v>
+      </c>
+      <c r="K23" t="s">
+        <v>145</v>
       </c>
       <c r="L23" t="s">
         <v>74</v>
       </c>
       <c r="M23" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B24">
-        <v>2012</v>
+        <v>1983</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
-        <v>160</v>
-      </c>
-      <c r="I24">
-        <v>1820</v>
+        <v>151</v>
+      </c>
+      <c r="H24" t="s">
+        <v>68</v>
+      </c>
+      <c r="I24" t="s">
+        <v>153</v>
       </c>
       <c r="J24" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="L24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M24" t="s">
         <v>26</v>
       </c>
       <c r="N24" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="B25">
-        <v>1994</v>
+        <v>2012</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>114</v>
       </c>
       <c r="D25" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="G25" t="s">
-        <v>164</v>
-      </c>
-      <c r="H25" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" t="s">
-        <v>166</v>
+        <v>158</v>
+      </c>
+      <c r="I25">
+        <v>1820</v>
       </c>
       <c r="J25" t="s">
-        <v>167</v>
-      </c>
-      <c r="K25" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="L25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M25" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="N25" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B26">
-        <v>1974</v>
+        <v>1994</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="F26" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="G26" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="H26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I26" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J26" t="s">
-        <v>154</v>
+        <v>165</v>
+      </c>
+      <c r="K26" t="s">
+        <v>163</v>
       </c>
       <c r="L26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M26" t="s">
-        <v>26</v>
-      </c>
-      <c r="N26" t="s">
-        <v>170</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B27">
-        <v>1987</v>
+        <v>1974</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="D27" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G27" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>37</v>
+      </c>
+      <c r="I27" t="s">
+        <v>167</v>
       </c>
       <c r="J27" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="L27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M27" t="s">
         <v>26</v>
       </c>
       <c r="N27" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>169</v>
+      </c>
+      <c r="B28">
+        <v>1987</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
+      <c r="G28" t="s">
+        <v>172</v>
+      </c>
+      <c r="H28" t="s">
+        <v>75</v>
+      </c>
+      <c r="J28" t="s">
+        <v>170</v>
+      </c>
+      <c r="L28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M28" t="s">
+        <v>26</v>
+      </c>
+      <c r="N28" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add tabular summaries of empirical results
</commit_message>
<xml_diff>
--- a/manuscript/Empirical Strategies Summary.xlsx
+++ b/manuscript/Empirical Strategies Summary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="189">
   <si>
     <t>Authors</t>
   </si>
@@ -290,9 +290,6 @@
     <t>1815-2001</t>
   </si>
   <si>
-    <t>Post 1945, NATO member, Milex/GDP, Milper / personnel, rivalry, lag alliance, democracy, prior conscription</t>
-  </si>
-  <si>
     <t>Focus on credibility of alliance commitment</t>
   </si>
   <si>
@@ -591,6 +588,9 @@
   </si>
   <si>
     <t>CONDITIONAL. Also robust, lots of different model specs and estimators show same result</t>
+  </si>
+  <si>
+    <t>Post 1945, NATO member, Milex/personnel, Milper / personnel, rivalry, lag alliance, democracy, prior conscription</t>
   </si>
 </sst>
 </file>
@@ -911,7 +911,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,34 +1017,34 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3">
         <v>1991</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3" t="s">
         <v>186</v>
-      </c>
-      <c r="G3" t="s">
-        <v>187</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L3" t="s">
         <v>73</v>
@@ -1104,6 +1104,9 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" t="s">
         <v>41</v>
       </c>
@@ -1249,7 +1252,7 @@
         <v>17</v>
       </c>
       <c r="N8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1295,7 +1298,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B10">
         <v>2003</v>
@@ -1304,25 +1307,25 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F10" t="s">
         <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H10" t="s">
         <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="L10" t="s">
         <v>74</v>
@@ -1336,7 +1339,7 @@
         <v>1990</v>
       </c>
       <c r="C11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" t="s">
         <v>78</v>
@@ -1351,7 +1354,7 @@
         <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I11" t="s">
         <v>71</v>
@@ -1401,7 +1404,7 @@
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>88</v>
+        <v>188</v>
       </c>
       <c r="L12" t="s">
         <v>74</v>
@@ -1410,12 +1413,12 @@
         <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13">
         <v>2010</v>
@@ -1433,19 +1436,19 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L13" t="s">
         <v>74</v>
@@ -1456,7 +1459,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14">
         <v>2000</v>
@@ -1471,22 +1474,22 @@
         <v>84</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H14" t="s">
         <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J14" t="s">
         <v>16</v>
       </c>
       <c r="K14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L14" t="s">
         <v>74</v>
@@ -1497,7 +1500,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B15">
         <v>2003</v>
@@ -1512,19 +1515,19 @@
         <v>41</v>
       </c>
       <c r="F15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" t="s">
         <v>94</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
       </c>
       <c r="H15" t="s">
         <v>37</v>
       </c>
       <c r="I15" t="s">
+        <v>95</v>
+      </c>
+      <c r="J15" t="s">
         <v>96</v>
-      </c>
-      <c r="J15" t="s">
-        <v>97</v>
       </c>
       <c r="L15" t="s">
         <v>74</v>
@@ -1533,39 +1536,39 @@
         <v>17</v>
       </c>
       <c r="N15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16">
         <v>1993</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" t="s">
         <v>100</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>101</v>
-      </c>
-      <c r="G16" t="s">
-        <v>102</v>
       </c>
       <c r="H16" t="s">
         <v>36</v>
       </c>
       <c r="I16" t="s">
+        <v>102</v>
+      </c>
+      <c r="J16" t="s">
         <v>103</v>
-      </c>
-      <c r="J16" t="s">
-        <v>104</v>
       </c>
       <c r="L16" t="s">
         <v>73</v>
@@ -1574,39 +1577,39 @@
         <v>17</v>
       </c>
       <c r="N16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17">
         <v>1987</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" t="s">
         <v>108</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>109</v>
-      </c>
-      <c r="G17" t="s">
-        <v>110</v>
       </c>
       <c r="H17" t="s">
         <v>68</v>
       </c>
       <c r="I17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K17" t="s">
         <v>68</v>
@@ -1618,30 +1621,30 @@
         <v>17</v>
       </c>
       <c r="N17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B18">
         <v>1966</v>
       </c>
       <c r="C18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
         <v>67</v>
       </c>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
         <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H18" t="s">
         <v>37</v>
@@ -1661,7 +1664,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B19">
         <v>1996</v>
@@ -1679,19 +1682,19 @@
         <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H19" t="s">
         <v>37</v>
       </c>
       <c r="I19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J19" t="s">
         <v>16</v>
       </c>
       <c r="K19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L19" t="s">
         <v>73</v>
@@ -1700,18 +1703,18 @@
         <v>26</v>
       </c>
       <c r="N19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20">
         <v>1990</v>
       </c>
       <c r="C20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D20" t="s">
         <v>22</v>
@@ -1723,19 +1726,19 @@
         <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H20" t="s">
         <v>37</v>
       </c>
       <c r="I20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J20" t="s">
         <v>72</v>
       </c>
       <c r="K20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L20" t="s">
         <v>73</v>
@@ -1744,12 +1747,12 @@
         <v>26</v>
       </c>
       <c r="N20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B21">
         <v>1999</v>
@@ -1758,25 +1761,25 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
       </c>
       <c r="F21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" t="s">
         <v>128</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" t="s">
         <v>129</v>
-      </c>
-      <c r="H21" t="s">
-        <v>131</v>
-      </c>
-      <c r="I21" t="s">
-        <v>96</v>
-      </c>
-      <c r="J21" t="s">
-        <v>130</v>
       </c>
       <c r="L21" t="s">
         <v>74</v>
@@ -1785,18 +1788,18 @@
         <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22">
         <v>2015</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
@@ -1808,19 +1811,19 @@
         <v>57</v>
       </c>
       <c r="G22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H22" t="s">
         <v>36</v>
       </c>
       <c r="I22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J22" t="s">
         <v>72</v>
       </c>
       <c r="K22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L22" t="s">
         <v>73</v>
@@ -1831,25 +1834,25 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B23">
         <v>2011</v>
       </c>
       <c r="C23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F23" t="s">
         <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H23" t="s">
         <v>37</v>
@@ -1858,10 +1861,10 @@
         <v>2000</v>
       </c>
       <c r="J23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L23" t="s">
         <v>74</v>
@@ -1870,39 +1873,39 @@
         <v>17</v>
       </c>
       <c r="N23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24">
         <v>1983</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D24" t="s">
         <v>22</v>
       </c>
       <c r="E24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" t="s">
         <v>150</v>
-      </c>
-      <c r="F24" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" t="s">
-        <v>151</v>
       </c>
       <c r="H24" t="s">
         <v>68</v>
       </c>
       <c r="I24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L24" t="s">
         <v>73</v>
@@ -1911,18 +1914,18 @@
         <v>26</v>
       </c>
       <c r="N24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B25">
         <v>2012</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D25" t="s">
         <v>22</v>
@@ -1934,13 +1937,13 @@
         <v>69</v>
       </c>
       <c r="G25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I25">
         <v>1820</v>
       </c>
       <c r="J25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L25" t="s">
         <v>73</v>
@@ -1949,12 +1952,12 @@
         <v>26</v>
       </c>
       <c r="N25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B26">
         <v>1994</v>
@@ -1966,25 +1969,25 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" t="s">
         <v>160</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>161</v>
-      </c>
-      <c r="G26" t="s">
-        <v>162</v>
       </c>
       <c r="H26" t="s">
         <v>36</v>
       </c>
       <c r="I26" t="s">
+        <v>163</v>
+      </c>
+      <c r="J26" t="s">
         <v>164</v>
       </c>
-      <c r="J26" t="s">
-        <v>165</v>
-      </c>
       <c r="K26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L26" t="s">
         <v>73</v>
@@ -1995,34 +1998,34 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B27">
         <v>1974</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s">
         <v>67</v>
       </c>
       <c r="E27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" t="s">
         <v>150</v>
-      </c>
-      <c r="F27" t="s">
-        <v>128</v>
-      </c>
-      <c r="G27" t="s">
-        <v>151</v>
       </c>
       <c r="H27" t="s">
         <v>37</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="J27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L27" t="s">
         <v>73</v>
@@ -2031,12 +2034,12 @@
         <v>26</v>
       </c>
       <c r="N27" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B28">
         <v>1987</v>
@@ -2051,16 +2054,16 @@
         <v>68</v>
       </c>
       <c r="F28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H28" t="s">
         <v>75</v>
       </c>
       <c r="J28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L28" t="s">
         <v>73</v>
@@ -2069,7 +2072,7 @@
         <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add section on substitution theory of foreign policy
</commit_message>
<xml_diff>
--- a/manuscript/Empirical Strategies Summary.xlsx
+++ b/manuscript/Empirical Strategies Summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="190">
   <si>
     <t>Authors</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t>Post 1945, NATO member, Milex/personnel, Milper / personnel, rivalry, lag alliance, democracy, prior conscription</t>
+  </si>
+  <si>
+    <t>State-specific time-series regs w/ Cochrane-Orcutt</t>
   </si>
 </sst>
 </file>
@@ -911,7 +914,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,6 +1134,9 @@
       <c r="M5" t="s">
         <v>17</v>
       </c>
+      <c r="N5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">

</xml_diff>

<commit_message>
Summarize cooperation model of complementarity
</commit_message>
<xml_diff>
--- a/manuscript/Empirical Strategies Summary.xlsx
+++ b/manuscript/Empirical Strategies Summary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="191">
   <si>
     <t>Authors</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Positive Coalition Mean: More conservative</t>
   </si>
   <si>
-    <t>Coalition Mean, GDP, split by size</t>
-  </si>
-  <si>
     <t>1950-1978</t>
   </si>
   <si>
@@ -594,6 +591,12 @@
   </si>
   <si>
     <t>State-specific time-series regs w/ Cochrane-Orcutt</t>
+  </si>
+  <si>
+    <t>Western European States</t>
+  </si>
+  <si>
+    <t>Coalition Mean, GNP, US defense buden, all split by size</t>
   </si>
 </sst>
 </file>
@@ -914,7 +917,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1020,7 +1023,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>1991</v>
@@ -1035,19 +1038,19 @@
         <v>99</v>
       </c>
       <c r="F3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G3" t="s">
         <v>185</v>
-      </c>
-      <c r="G3" t="s">
-        <v>186</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
       </c>
       <c r="I3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L3" t="s">
         <v>73</v>
@@ -1135,7 +1138,7 @@
         <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1258,7 +1261,7 @@
         <v>17</v>
       </c>
       <c r="N8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1304,7 +1307,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10">
         <v>2003</v>
@@ -1313,25 +1316,25 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F10" t="s">
         <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H10" t="s">
         <v>68</v>
       </c>
       <c r="I10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J10" t="s">
         <v>16</v>
       </c>
       <c r="K10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L10" t="s">
         <v>74</v>
@@ -1360,7 +1363,7 @@
         <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I11" t="s">
         <v>71</v>
@@ -1410,7 +1413,7 @@
         <v>16</v>
       </c>
       <c r="K12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L12" t="s">
         <v>74</v>
@@ -1424,7 +1427,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B13">
         <v>2010</v>
@@ -1442,19 +1445,19 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H13" t="s">
         <v>37</v>
       </c>
       <c r="I13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="J13" t="s">
         <v>16</v>
       </c>
       <c r="K13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L13" t="s">
         <v>74</v>
@@ -1465,7 +1468,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14">
         <v>2000</v>
@@ -1506,7 +1509,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15">
         <v>2003</v>
@@ -1542,7 +1545,7 @@
         <v>17</v>
       </c>
       <c r="N15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -1588,7 +1591,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17">
         <v>1987</v>
@@ -1632,7 +1635,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B18">
         <v>1966</v>
@@ -1670,7 +1673,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B19">
         <v>1996</v>
@@ -1732,16 +1735,16 @@
         <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
+        <v>190</v>
       </c>
       <c r="H20" t="s">
         <v>37</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J20" t="s">
-        <v>72</v>
+        <v>189</v>
       </c>
       <c r="K20" t="s">
         <v>122</v>
@@ -1753,12 +1756,12 @@
         <v>26</v>
       </c>
       <c r="N20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B21">
         <v>1999</v>
@@ -1767,25 +1770,25 @@
         <v>32</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
         <v>41</v>
       </c>
       <c r="F21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" t="s">
         <v>127</v>
       </c>
-      <c r="G21" t="s">
-        <v>128</v>
-      </c>
       <c r="H21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I21" t="s">
         <v>95</v>
       </c>
       <c r="J21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L21" t="s">
         <v>74</v>
@@ -1794,18 +1797,18 @@
         <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22">
         <v>2015</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
@@ -1817,19 +1820,19 @@
         <v>57</v>
       </c>
       <c r="G22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H22" t="s">
         <v>36</v>
       </c>
       <c r="I22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J22" t="s">
         <v>72</v>
       </c>
       <c r="K22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L22" t="s">
         <v>73</v>
@@ -1840,25 +1843,25 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B23">
         <v>2011</v>
       </c>
       <c r="C23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
         <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H23" t="s">
         <v>37</v>
@@ -1867,10 +1870,10 @@
         <v>2000</v>
       </c>
       <c r="J23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L23" t="s">
         <v>74</v>
@@ -1879,12 +1882,12 @@
         <v>17</v>
       </c>
       <c r="N23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B24">
         <v>1983</v>
@@ -1896,22 +1899,22 @@
         <v>22</v>
       </c>
       <c r="E24" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" t="s">
+        <v>126</v>
+      </c>
+      <c r="G24" t="s">
         <v>149</v>
-      </c>
-      <c r="F24" t="s">
-        <v>127</v>
-      </c>
-      <c r="G24" t="s">
-        <v>150</v>
       </c>
       <c r="H24" t="s">
         <v>68</v>
       </c>
       <c r="I24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L24" t="s">
         <v>73</v>
@@ -1920,12 +1923,12 @@
         <v>26</v>
       </c>
       <c r="N24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B25">
         <v>2012</v>
@@ -1943,13 +1946,13 @@
         <v>69</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I25">
         <v>1820</v>
       </c>
       <c r="J25" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L25" t="s">
         <v>73</v>
@@ -1958,12 +1961,12 @@
         <v>26</v>
       </c>
       <c r="N25" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26">
         <v>1994</v>
@@ -1975,25 +1978,25 @@
         <v>12</v>
       </c>
       <c r="E26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" t="s">
         <v>159</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>160</v>
-      </c>
-      <c r="G26" t="s">
-        <v>161</v>
       </c>
       <c r="H26" t="s">
         <v>36</v>
       </c>
       <c r="I26" t="s">
+        <v>162</v>
+      </c>
+      <c r="J26" t="s">
         <v>163</v>
       </c>
-      <c r="J26" t="s">
-        <v>164</v>
-      </c>
       <c r="K26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L26" t="s">
         <v>73</v>
@@ -2004,7 +2007,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27">
         <v>1974</v>
@@ -2016,22 +2019,22 @@
         <v>67</v>
       </c>
       <c r="E27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F27" t="s">
+        <v>126</v>
+      </c>
+      <c r="G27" t="s">
         <v>149</v>
-      </c>
-      <c r="F27" t="s">
-        <v>127</v>
-      </c>
-      <c r="G27" t="s">
-        <v>150</v>
       </c>
       <c r="H27" t="s">
         <v>37</v>
       </c>
       <c r="I27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="L27" t="s">
         <v>73</v>
@@ -2040,12 +2043,12 @@
         <v>26</v>
       </c>
       <c r="N27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B28">
         <v>1987</v>
@@ -2060,16 +2063,16 @@
         <v>68</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H28" t="s">
         <v>75</v>
       </c>
       <c r="J28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L28" t="s">
         <v>73</v>
@@ -2078,7 +2081,7 @@
         <v>26</v>
       </c>
       <c r="N28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>